<commit_message>
validate data when login and change pasword
</commit_message>
<xml_diff>
--- a/password.xlsx
+++ b/password.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/24b330371c0187a5/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PTIT\SQA\electricitySystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{AAF34508-B32F-4A34-809D-40BF6A1D627C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BE1242B-B6CB-483B-AF65-0EC48693AAC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2B28D1-E31B-48D7-8EAE-EC6E07D8DE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2748" yWindow="3108" windowWidth="17280" windowHeight="8880" xr2:uid="{E1BC5642-9394-49A8-993F-4FE3E891EA18}"/>
   </bookViews>
@@ -34,50 +34,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
-  <si>
-    <t>ESHNHD001</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>ESHNHD002</t>
-  </si>
-  <si>
     <t>67hgQFls</t>
   </si>
   <si>
     <t>df29mOPt</t>
   </si>
   <si>
-    <t>ESHNHD003</t>
-  </si>
-  <si>
-    <t>ESHNHD006</t>
-  </si>
-  <si>
     <t>mk34esBL</t>
   </si>
   <si>
     <t>8hmkTEwr</t>
   </si>
   <si>
-    <t>ESHNHD005</t>
-  </si>
-  <si>
-    <t>ESHNHD004</t>
-  </si>
-  <si>
     <t>45ErbheL</t>
   </si>
   <si>
     <t>Refb45t0</t>
   </si>
   <si>
-    <t>ESHNHD007</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -88,6 +67,36 @@
   </si>
   <si>
     <t>bichdiep</t>
+  </si>
+  <si>
+    <t>HD11300002</t>
+  </si>
+  <si>
+    <t>HD11300001</t>
+  </si>
+  <si>
+    <t>HD11300003</t>
+  </si>
+  <si>
+    <t>HD11300004</t>
+  </si>
+  <si>
+    <t>HD11300005</t>
+  </si>
+  <si>
+    <t>HD11300006</t>
+  </si>
+  <si>
+    <t>HD11300007</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>ngochoai123</t>
+  </si>
+  <si>
+    <t>bichdiep123</t>
   </si>
 </sst>
 </file>
@@ -442,122 +451,123 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>